<commit_message>
error in current balance calculation finxed
</commit_message>
<xml_diff>
--- a/afar_project/csv_path/excel_files/frc_asset_schedule.xlsx
+++ b/afar_project/csv_path/excel_files/frc_asset_schedule.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -555,7 +555,7 @@
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
@@ -667,7 +667,7 @@
       </c>
       <c r="P4" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
@@ -723,7 +723,7 @@
       </c>
       <c r="P5" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
@@ -779,7 +779,7 @@
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
@@ -835,7 +835,7 @@
       </c>
       <c r="P7" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
@@ -891,7 +891,7 @@
       </c>
       <c r="P8" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
@@ -947,7 +947,7 @@
       </c>
       <c r="P9" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="P10" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
@@ -1059,7 +1059,7 @@
       </c>
       <c r="P11" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
@@ -1115,7 +1115,7 @@
       </c>
       <c r="P12" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
@@ -1171,7 +1171,7 @@
       </c>
       <c r="P13" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
@@ -1227,7 +1227,7 @@
       </c>
       <c r="P14" t="inlineStr">
         <is>
-          <t> </t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>

</xml_diff>